<commit_message>
added ksom wallFollow 01 hold 2 xls file 2
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_wallFollow_01_hold_02.xlsx
+++ b/results_analysis/ksom_wallFollow_01_hold_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BFCCC4-032C-45EB-A8C6-9BDF341917F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C2ADC-DF28-4E39-A66A-C13EF03722A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="hp_best" sheetId="7" r:id="rId1"/>
@@ -115,8 +115,16 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -449,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,6 +495,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -514,6 +528,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,24 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -928,9 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F67E61-AD41-41B7-8D96-4B4B381E1959}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -950,29 +953,29 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="40" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="40" t="s">
+      <c r="M2" s="46"/>
+      <c r="N2" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="42"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -981,43 +984,43 @@
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1028,57 +1031,135 @@
       <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="4"/>
+      <c r="C4" s="38">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="D4" s="20">
+        <v>32</v>
+      </c>
+      <c r="E4" s="35">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="F4" s="20">
+        <v>256</v>
+      </c>
+      <c r="G4" s="20">
+        <v>1</v>
+      </c>
+      <c r="H4" s="20">
+        <v>1024</v>
+      </c>
+      <c r="I4" s="20">
+        <v>32</v>
+      </c>
+      <c r="J4" s="20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K4" s="20">
+        <v>32</v>
+      </c>
+      <c r="L4" s="35">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="M4" s="35">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="N4" s="20">
+        <v>256</v>
+      </c>
+      <c r="O4" s="4">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="21"/>
+      <c r="C5" s="21">
+        <v>512</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="22">
+        <v>4</v>
+      </c>
+      <c r="F5" s="22">
+        <v>64</v>
+      </c>
+      <c r="G5" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="H5" s="22">
+        <v>32</v>
+      </c>
+      <c r="I5" s="22">
+        <v>1</v>
+      </c>
+      <c r="J5" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="K5" s="22">
+        <v>32</v>
+      </c>
+      <c r="L5" s="36">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="M5" s="36">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="N5" s="22">
+        <v>1</v>
+      </c>
+      <c r="O5" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="21"/>
+      <c r="C6" s="39">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D6" s="22">
+        <v>16</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="22">
+        <v>512</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="22">
+        <v>8</v>
+      </c>
+      <c r="I6" s="22">
+        <v>16</v>
+      </c>
+      <c r="J6" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="K6" s="22">
+        <v>16</v>
+      </c>
+      <c r="L6" s="36">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="M6" s="36">
+        <v>-3.125E-2</v>
+      </c>
+      <c r="N6" s="22">
+        <v>2</v>
+      </c>
+      <c r="O6" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -1087,57 +1168,135 @@
       <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="21"/>
+      <c r="C7" s="39">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D7" s="22">
+        <v>32</v>
+      </c>
+      <c r="E7" s="36">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="F7" s="22">
+        <v>64</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="H7" s="22">
+        <v>1</v>
+      </c>
+      <c r="I7" s="22">
+        <v>32</v>
+      </c>
+      <c r="J7" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="K7" s="22">
+        <v>32</v>
+      </c>
+      <c r="L7" s="36">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="M7" s="36">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="N7" s="22">
+        <v>16</v>
+      </c>
+      <c r="O7" s="23">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="21"/>
+      <c r="C8" s="21">
+        <v>1024</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0.125</v>
+      </c>
+      <c r="F8" s="22">
+        <v>32</v>
+      </c>
+      <c r="G8" s="22">
+        <v>1</v>
+      </c>
+      <c r="H8" s="22">
+        <v>256</v>
+      </c>
+      <c r="I8" s="22">
+        <v>16</v>
+      </c>
+      <c r="J8" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="22">
+        <v>2</v>
+      </c>
+      <c r="L8" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="M8" s="22">
+        <v>1</v>
+      </c>
+      <c r="N8" s="36">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="O8" s="23">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="23"/>
+      <c r="C9" s="40">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="D9" s="24">
+        <v>8</v>
+      </c>
+      <c r="E9" s="37">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="F9" s="24">
+        <v>1</v>
+      </c>
+      <c r="G9" s="24">
+        <v>1</v>
+      </c>
+      <c r="H9" s="24">
+        <v>1024</v>
+      </c>
+      <c r="I9" s="24">
+        <v>32</v>
+      </c>
+      <c r="J9" s="24">
+        <v>2</v>
+      </c>
+      <c r="K9" s="24">
+        <v>32</v>
+      </c>
+      <c r="L9" s="37">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="M9" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="N9" s="37">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="O9" s="25">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1168,18 +1327,18 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -1220,42 +1379,90 @@
       <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25"/>
+      <c r="C4" s="29">
+        <v>0.62026431718061703</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.79383259911894299</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.79361233480176196</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0.78788546255506597</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0.79537444933920698</v>
+      </c>
+      <c r="H4" s="29">
+        <v>0.79515418502202595</v>
+      </c>
+      <c r="I4" s="29">
+        <v>0.80726872246696002</v>
+      </c>
+      <c r="J4" s="30">
+        <v>0.808810572687225</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
+      <c r="C5" s="31">
+        <v>0.61277533039647603</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.62246696035242299</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0.61409691629955898</v>
+      </c>
+      <c r="F5" s="31">
+        <v>0.78590308370044104</v>
+      </c>
+      <c r="G5" s="31">
+        <v>0.82665198237885495</v>
+      </c>
+      <c r="H5" s="31">
+        <v>0.79977973568281902</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0.60837004405286299</v>
+      </c>
+      <c r="J5" s="32">
+        <v>0.61167400881057299</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
+      <c r="C6" s="31">
+        <v>0.74911894273127799</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.80220264317180601</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0.79735682819383302</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.79933920704845796</v>
+      </c>
+      <c r="G6" s="31">
+        <v>0.81145374449339203</v>
+      </c>
+      <c r="H6" s="31">
+        <v>0.81079295154185005</v>
+      </c>
+      <c r="I6" s="31">
+        <v>0.79845814977973595</v>
+      </c>
+      <c r="J6" s="32">
+        <v>0.82863436123348</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -1264,57 +1471,105 @@
       <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
+      <c r="C7" s="31">
+        <v>0.61696035242290803</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.79735682819383302</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.790528634361233</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.79757709251101305</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.77973568281938299</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0.81057268722467002</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0.8</v>
+      </c>
+      <c r="J7" s="32">
+        <v>0.798017621145374</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="31">
+        <v>0.73920704845815</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.66872246696035198</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0.61409691629955898</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0.78546255506607898</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.610132158590308</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0.60638766519823795</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0.72290748898678403</v>
+      </c>
+      <c r="J8" s="32">
+        <v>0.61740088105726898</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="C9" s="33">
+        <v>0.736784140969163</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.80176211453744495</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0.80154185022026403</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0.788105726872247</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.80044052863436099</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0.78876651982378898</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0.79030837004405297</v>
+      </c>
+      <c r="J9" s="34">
+        <v>0.79295154185021999</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -1355,42 +1610,90 @@
       <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="C13" s="29">
+        <v>0.75352422907489003</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.80528634361233498</v>
+      </c>
+      <c r="E13" s="29">
+        <v>0.81101321585903097</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0.80572687224669604</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0.80837004405286295</v>
+      </c>
+      <c r="H13" s="29">
+        <v>0.81057268722467002</v>
+      </c>
+      <c r="I13" s="29">
+        <v>0.804625550660793</v>
+      </c>
+      <c r="J13" s="30">
+        <v>0.81497797356828205</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="C14" s="31">
+        <v>0.73303964757709295</v>
+      </c>
+      <c r="D14" s="31">
+        <v>0.82577092511013195</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.61563876651982397</v>
+      </c>
+      <c r="F14" s="31">
+        <v>0.78193832599118895</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.80264317180616696</v>
+      </c>
+      <c r="H14" s="31">
+        <v>0.80374449339206999</v>
+      </c>
+      <c r="I14" s="31">
+        <v>0.61607929515418502</v>
+      </c>
+      <c r="J14" s="32">
+        <v>0.76453744493392095</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="C15" s="31">
+        <v>0.75837004405286401</v>
+      </c>
+      <c r="D15" s="31">
+        <v>0.81607929515418498</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.81013215859030796</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.79691629955947096</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.81365638766519799</v>
+      </c>
+      <c r="H15" s="31">
+        <v>0.81189427312775297</v>
+      </c>
+      <c r="I15" s="31">
+        <v>0.81145374449339203</v>
+      </c>
+      <c r="J15" s="32">
+        <v>0.83237885462555095</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -1399,42 +1702,90 @@
       <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
+      <c r="C16" s="31">
+        <v>0.75176211453744501</v>
+      </c>
+      <c r="D16" s="31">
+        <v>0.75903083700440499</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.777312775330396</v>
+      </c>
+      <c r="F16" s="31">
+        <v>0.63215859030836996</v>
+      </c>
+      <c r="G16" s="31">
+        <v>0.76255506607929502</v>
+      </c>
+      <c r="H16" s="31">
+        <v>0.75044052863436095</v>
+      </c>
+      <c r="I16" s="31">
+        <v>0.76035242290748895</v>
+      </c>
+      <c r="J16" s="32">
+        <v>0.63480176211453698</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="C17" s="31">
+        <v>0.75550660792951496</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.753303964757709</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0.74185022026431702</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.73568281938325997</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.756607929515419</v>
+      </c>
+      <c r="H17" s="31">
+        <v>0.74713656387665195</v>
+      </c>
+      <c r="I17" s="31">
+        <v>0.75044052863436095</v>
+      </c>
+      <c r="J17" s="32">
+        <v>0.764096916299559</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
+      <c r="C18" s="33">
+        <v>0.76982378854625599</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0.75286343612334805</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0.75352422907489003</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0.76101321585903103</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0.75616740088105705</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0.77621145374449296</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0.75066079295154198</v>
+      </c>
+      <c r="J18" s="34">
+        <v>0.76828193832599101</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1449,9 +1800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C2E4AB-28B4-4560-9CA9-8AF5549FD7E4}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:J18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1462,18 +1811,18 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -1508,107 +1857,203 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="C4" s="29">
+        <v>0.60354625550660801</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.70400881057268705</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.66273127753303995</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0.69662995594713695</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0.69557268722467003</v>
+      </c>
+      <c r="H4" s="26">
+        <v>0.71819383259911895</v>
+      </c>
+      <c r="I4" s="26">
+        <v>0.73255506607929499</v>
+      </c>
+      <c r="J4" s="27">
+        <v>0.73321585903083697</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47"/>
+      <c r="C5" s="31">
+        <v>0.42028634361233502</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.45640969162995598</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0.39442731277533</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0.66383259911894299</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0.53801762114537399</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0.58088105726872197</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0.49696035242290798</v>
+      </c>
+      <c r="J5" s="32">
+        <v>0.475594713656388</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
+      <c r="C6" s="31">
+        <v>0.58273127753303999</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.72253303964757698</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.75160792951541899</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.73191629955947102</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0.76182819383259903</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0.750814977973568</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0.75107929515418503</v>
+      </c>
+      <c r="J6" s="32">
+        <v>0.74870044052863405</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="41" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="47"/>
+      <c r="C7" s="31">
+        <v>0.600132158590308</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.704493392070485</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.75149779735682798</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.67484581497797402</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0.72259911894273099</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0.71737885462555095</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0.70819383259911906</v>
+      </c>
+      <c r="J7" s="28">
+        <v>0.74707048458149805</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="47"/>
+      <c r="C8" s="31">
+        <v>0.48066079295154202</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.46651982378854601</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.49903083700440498</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0.673039647577093</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.51165198237885501</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0.41129955947136598</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0.48790748898678399</v>
+      </c>
+      <c r="J8" s="32">
+        <v>0.44079295154185</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="38"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="49"/>
+      <c r="C9" s="33">
+        <v>0.49343612334801801</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.78266519823788505</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.76174008810572702</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0.69215859030837001</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.71541850220264303</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0.72156387665198196</v>
+      </c>
+      <c r="I9" s="16">
+        <v>0.75812775330396498</v>
+      </c>
+      <c r="J9" s="34">
+        <v>0.75229074889867797</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -1649,42 +2094,90 @@
       <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="C13" s="29">
+        <v>0.60968502202643204</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.77968942731277502</v>
+      </c>
+      <c r="E13" s="29">
+        <v>0.77281718061673998</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0.76540748898678401</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0.77552202643171797</v>
+      </c>
+      <c r="H13" s="29">
+        <v>0.77419162995594704</v>
+      </c>
+      <c r="I13" s="29">
+        <v>0.77800660792951604</v>
+      </c>
+      <c r="J13" s="30">
+        <v>0.77146916299559498</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="C14" s="31">
+        <v>0.49537665198237901</v>
+      </c>
+      <c r="D14" s="31">
+        <v>0.53148678414096895</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.47322687224669602</v>
+      </c>
+      <c r="F14" s="31">
+        <v>0.60663215859030795</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.51273788546255505</v>
+      </c>
+      <c r="H14" s="31">
+        <v>0.51921365638766503</v>
+      </c>
+      <c r="I14" s="31">
+        <v>0.43001762114537401</v>
+      </c>
+      <c r="J14" s="32">
+        <v>0.50853964757709302</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="C15" s="31">
+        <v>0.58631497797356802</v>
+      </c>
+      <c r="D15" s="31">
+        <v>0.76479955947136602</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.76504405286343602</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.70205947136563895</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.75740528634361204</v>
+      </c>
+      <c r="H15" s="31">
+        <v>0.753162995594714</v>
+      </c>
+      <c r="I15" s="31">
+        <v>0.78784801762114498</v>
+      </c>
+      <c r="J15" s="32">
+        <v>0.603665198237885</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
@@ -1693,42 +2186,90 @@
       <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
+      <c r="C16" s="31">
+        <v>0.60774229074889896</v>
+      </c>
+      <c r="D16" s="31">
+        <v>0.60589867841409695</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.60850220264317201</v>
+      </c>
+      <c r="F16" s="31">
+        <v>0.60886784140969197</v>
+      </c>
+      <c r="G16" s="31">
+        <v>0.60683259911894305</v>
+      </c>
+      <c r="H16" s="31">
+        <v>0.60707709251101305</v>
+      </c>
+      <c r="I16" s="31">
+        <v>0.60851982378854597</v>
+      </c>
+      <c r="J16" s="32">
+        <v>0.60542731277533102</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="C17" s="31">
+        <v>0.48772466960352401</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.48175330396475802</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0.46383039647577101</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.51148678414096904</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.46964537444933901</v>
+      </c>
+      <c r="H17" s="31">
+        <v>0.48463436123348003</v>
+      </c>
+      <c r="I17" s="31">
+        <v>0.479909691629956</v>
+      </c>
+      <c r="J17" s="32">
+        <v>0.50255286343612304</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="39"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
+      <c r="C18" s="33">
+        <v>0.52212334801762095</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0.57534581497797399</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0.559011013215859</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0.56632819383259903</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0.52394273127753299</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0.57229295154185</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0.58250220264317198</v>
+      </c>
+      <c r="J18" s="34">
+        <v>0.553077092511013</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1743,9 +2284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C1C768-E5FF-4F1E-85F6-B83F97AC222C}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:J18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1755,18 +2294,18 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -1807,42 +2346,90 @@
       <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25"/>
+      <c r="C4" s="29">
+        <v>0.61101321585903101</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.74988986784140998</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.74129955947136605</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0.69129955947136601</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0.72378854625550704</v>
+      </c>
+      <c r="H4" s="29">
+        <v>0.73634361233480194</v>
+      </c>
+      <c r="I4" s="29">
+        <v>0.78160792951541902</v>
+      </c>
+      <c r="J4" s="30">
+        <v>0.75308370044052897</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
+      <c r="C5" s="31">
+        <v>0.34878854625550698</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.46002202643171802</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0.33083700440528602</v>
+      </c>
+      <c r="F5" s="31">
+        <v>0.66541850220264298</v>
+      </c>
+      <c r="G5" s="31">
+        <v>0.51310572687224698</v>
+      </c>
+      <c r="H5" s="31">
+        <v>0.61079295154184998</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0.53248898678414103</v>
+      </c>
+      <c r="J5" s="32">
+        <v>0.55517621145374396</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
+      <c r="C6" s="31">
+        <v>0.60781938325991203</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.74526431718061703</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0.76167400881057301</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.77037444933920696</v>
+      </c>
+      <c r="G6" s="31">
+        <v>0.75770925110132203</v>
+      </c>
+      <c r="H6" s="31">
+        <v>0.78017621145374505</v>
+      </c>
+      <c r="I6" s="31">
+        <v>0.77433920704845804</v>
+      </c>
+      <c r="J6" s="32">
+        <v>0.77444933920704795</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -1851,57 +2438,105 @@
       <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
+      <c r="C7" s="31">
+        <v>0.60748898678414098</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.70914096916299596</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.77808370044052899</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.62323788546255499</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.772356828193833</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0.77037444933920696</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0.75143171806167397</v>
+      </c>
+      <c r="J7" s="32">
+        <v>0.77709251101321597</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="31">
+        <v>0.41949339207048503</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.50253303964757701</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0.52577092511013201</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0.706938325991189</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.60484581497797396</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0.45605726872246699</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0.46751101321585897</v>
+      </c>
+      <c r="J8" s="32">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="C9" s="33">
+        <v>0.452422907488987</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.79449339207048497</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0.78259911894273104</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0.67235682819383302</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.75781938325991205</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0.76101321585903103</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0.76508810572687203</v>
+      </c>
+      <c r="J9" s="34">
+        <v>0.75892070484581498</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -1942,42 +2577,90 @@
       <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="C13" s="29">
+        <v>0.60969162995594695</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.78909691629956003</v>
+      </c>
+      <c r="E13" s="29">
+        <v>0.78149779735682801</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0.784801762114537</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0.783920704845815</v>
+      </c>
+      <c r="H13" s="29">
+        <v>0.78270925110132195</v>
+      </c>
+      <c r="I13" s="29">
+        <v>0.78678414096916305</v>
+      </c>
+      <c r="J13" s="30">
+        <v>0.78116740088105696</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="C14" s="31">
+        <v>0.48149779735682802</v>
+      </c>
+      <c r="D14" s="31">
+        <v>0.54284140969162997</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.36971365638766501</v>
+      </c>
+      <c r="F14" s="31">
+        <v>0.61266519823788601</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.54328193832599103</v>
+      </c>
+      <c r="H14" s="31">
+        <v>0.46971365638766499</v>
+      </c>
+      <c r="I14" s="31">
+        <v>0.35825991189427298</v>
+      </c>
+      <c r="J14" s="32">
+        <v>0.54063876651982401</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="C15" s="31">
+        <v>0.61629955947136605</v>
+      </c>
+      <c r="D15" s="31">
+        <v>0.76354625550660804</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.75638766519823797</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.743392070484581</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.74856828193832603</v>
+      </c>
+      <c r="H15" s="31">
+        <v>0.74647577092510997</v>
+      </c>
+      <c r="I15" s="31">
+        <v>0.78909691629956003</v>
+      </c>
+      <c r="J15" s="32">
+        <v>0.60704845814978003</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
@@ -1986,42 +2669,90 @@
       <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
+      <c r="C16" s="31">
+        <v>0.61101321585903101</v>
+      </c>
+      <c r="D16" s="31">
+        <v>0.61068281938325997</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.61167400881057299</v>
+      </c>
+      <c r="F16" s="31">
+        <v>0.610903083700441</v>
+      </c>
+      <c r="G16" s="31">
+        <v>0.61079295154184998</v>
+      </c>
+      <c r="H16" s="31">
+        <v>0.61035242290748903</v>
+      </c>
+      <c r="I16" s="31">
+        <v>0.60991189427312797</v>
+      </c>
+      <c r="J16" s="32">
+        <v>0.61057268722466995</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="C17" s="31">
+        <v>0.455726872246696</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.45363436123348</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0.45308370044052898</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.54955947136563899</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.45330396475770901</v>
+      </c>
+      <c r="H17" s="31">
+        <v>0.45550660792951497</v>
+      </c>
+      <c r="I17" s="31">
+        <v>0.45440528634361199</v>
+      </c>
+      <c r="J17" s="32">
+        <v>0.45638766519823798</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
+      <c r="C18" s="33">
+        <v>0.45462555066079302</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0.61035242290748903</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0.60837004405286299</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0.60914096916299598</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0.45550660792951497</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0.61145374449339196</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0.60947136563876703</v>
+      </c>
+      <c r="J18" s="34">
+        <v>0.59361233480176201</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2036,9 +2767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31608D6-694E-4C0B-957B-CCC750DA682C}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:J18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2048,18 +2777,18 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -2100,42 +2829,90 @@
       <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25"/>
+      <c r="C4" s="29">
+        <v>2.5014943966047601E-2</v>
+      </c>
+      <c r="D4" s="29">
+        <v>9.8075587692774996E-2</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.23903381660265699</v>
+      </c>
+      <c r="F4" s="29">
+        <v>8.3178879031959099E-2</v>
+      </c>
+      <c r="G4" s="29">
+        <v>9.8722514466403705E-2</v>
+      </c>
+      <c r="H4" s="29">
+        <v>8.3499914365174704E-2</v>
+      </c>
+      <c r="I4" s="29">
+        <v>8.6402204739379901E-2</v>
+      </c>
+      <c r="J4" s="30">
+        <v>6.43209353935211E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
+      <c r="C5" s="31">
+        <v>0.14262807441350001</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.14953852658674699</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0.108116754983799</v>
+      </c>
+      <c r="F5" s="31">
+        <v>7.4873871776447207E-2</v>
+      </c>
+      <c r="G5" s="31">
+        <v>0.16148958980900899</v>
+      </c>
+      <c r="H5" s="31">
+        <v>0.16711238246454599</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0.12097998767271501</v>
+      </c>
+      <c r="J5" s="32">
+        <v>0.173934251701958</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
+      <c r="C6" s="31">
+        <v>0.12138285804827</v>
+      </c>
+      <c r="D6" s="31">
+        <v>7.2212816483470901E-2</v>
+      </c>
+      <c r="E6" s="31">
+        <v>5.3215203622950701E-2</v>
+      </c>
+      <c r="F6" s="31">
+        <v>6.8063570900894405E-2</v>
+      </c>
+      <c r="G6" s="31">
+        <v>3.4338956657989403E-2</v>
+      </c>
+      <c r="H6" s="31">
+        <v>7.6335634980169501E-2</v>
+      </c>
+      <c r="I6" s="31">
+        <v>7.3942530427230896E-2</v>
+      </c>
+      <c r="J6" s="32">
+        <v>8.7806973294354995E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -2144,57 +2921,105 @@
       <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
+      <c r="C7" s="31">
+        <v>2.0482660344966999E-2</v>
+      </c>
+      <c r="D7" s="31">
+        <v>8.68168204010802E-2</v>
+      </c>
+      <c r="E7" s="31">
+        <v>5.9903507806109403E-2</v>
+      </c>
+      <c r="F7" s="31">
+        <v>9.0830884558982194E-2</v>
+      </c>
+      <c r="G7" s="31">
+        <v>9.6440908999504693E-2</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0.10644065072987199</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0.10725612299000099</v>
+      </c>
+      <c r="J7" s="32">
+        <v>7.9679958379958601E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="31">
+        <v>0.14949015368152899</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.16044457664066999</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0.118621109373117</v>
+      </c>
+      <c r="F8" s="31">
+        <v>8.9081672559562897E-2</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.12421034710588599</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0.13233818967984701</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0.111005613663358</v>
+      </c>
+      <c r="J8" s="32">
+        <v>0.148471831245376</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="C9" s="33">
+        <v>0.115946368500179</v>
+      </c>
+      <c r="D9" s="33">
+        <v>3.2601938270222203E-2</v>
+      </c>
+      <c r="E9" s="33">
+        <v>6.0776460516971803E-2</v>
+      </c>
+      <c r="F9" s="33">
+        <v>8.1250182765519402E-2</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.136432799899491</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0.12518169974641499</v>
+      </c>
+      <c r="I9" s="33">
+        <v>3.0453253420055601E-2</v>
+      </c>
+      <c r="J9" s="34">
+        <v>3.3138569484302702E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -2235,42 +3060,90 @@
       <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="C13" s="29">
+        <v>3.03315694898777E-2</v>
+      </c>
+      <c r="D13" s="29">
+        <v>2.60550350833267E-2</v>
+      </c>
+      <c r="E13" s="29">
+        <v>3.6290561786337501E-2</v>
+      </c>
+      <c r="F13" s="29">
+        <v>5.2238002990687198E-2</v>
+      </c>
+      <c r="G13" s="29">
+        <v>3.4661362174820701E-2</v>
+      </c>
+      <c r="H13" s="29">
+        <v>3.1374589164710101E-2</v>
+      </c>
+      <c r="I13" s="29">
+        <v>3.2836041458227598E-2</v>
+      </c>
+      <c r="J13" s="30">
+        <v>4.06699040450198E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="C14" s="31">
+        <v>0.111207998916815</v>
+      </c>
+      <c r="D14" s="31">
+        <v>0.163674065694001</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.127141599060063</v>
+      </c>
+      <c r="F14" s="31">
+        <v>3.9835270865886098E-2</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.151047301717327</v>
+      </c>
+      <c r="H14" s="31">
+        <v>0.122410652255596</v>
+      </c>
+      <c r="I14" s="31">
+        <v>0.12229060303030601</v>
+      </c>
+      <c r="J14" s="32">
+        <v>0.149088005815424</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="C15" s="31">
+        <v>0.137732964782949</v>
+      </c>
+      <c r="D15" s="31">
+        <v>3.4570998042945701E-2</v>
+      </c>
+      <c r="E15" s="31">
+        <v>2.8390855398232599E-2</v>
+      </c>
+      <c r="F15" s="31">
+        <v>8.3986117312546002E-2</v>
+      </c>
+      <c r="G15" s="31">
+        <v>2.1114476398411498E-2</v>
+      </c>
+      <c r="H15" s="31">
+        <v>2.52807815456015E-2</v>
+      </c>
+      <c r="I15" s="31">
+        <v>8.7081920918355201E-3</v>
+      </c>
+      <c r="J15" s="32">
+        <v>0.119481264849919</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
@@ -2279,42 +3152,90 @@
       <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
+      <c r="C16" s="31">
+        <v>3.8372894605937E-2</v>
+      </c>
+      <c r="D16" s="31">
+        <v>2.47261261216612E-2</v>
+      </c>
+      <c r="E16" s="31">
+        <v>2.5462953079996901E-2</v>
+      </c>
+      <c r="F16" s="31">
+        <v>1.39278402737793E-2</v>
+      </c>
+      <c r="G16" s="31">
+        <v>2.4567683236784699E-2</v>
+      </c>
+      <c r="H16" s="31">
+        <v>2.3866714560250399E-2</v>
+      </c>
+      <c r="I16" s="31">
+        <v>2.8215289081021101E-2</v>
+      </c>
+      <c r="J16" s="32">
+        <v>2.1485105342414001E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="C17" s="31">
+        <v>0.13561130729653201</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.12721928290863199</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0.123739740613673</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.12702732028292099</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.13381344879172</v>
+      </c>
+      <c r="H17" s="31">
+        <v>0.13106204231913299</v>
+      </c>
+      <c r="I17" s="31">
+        <v>0.12670222322703101</v>
+      </c>
+      <c r="J17" s="32">
+        <v>0.129166579408311</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
+      <c r="C18" s="33">
+        <v>0.13601548557231899</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0.13007017438855001</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0.13889614610322801</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0.134391728019816</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0.13588091590919801</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0.14595141327368299</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0.11977478722092801</v>
+      </c>
+      <c r="J18" s="34">
+        <v>0.15004155808608599</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2329,9 +3250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF95E80-F9D6-4C97-A976-8D8517BE58EB}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:J18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2341,18 +3260,18 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -2393,42 +3312,90 @@
       <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25"/>
+      <c r="C4" s="29">
+        <v>0.61886764094957802</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.766643748569942</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.76160647932622405</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0.74307472086943305</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0.75952790098161405</v>
+      </c>
+      <c r="H4" s="29">
+        <v>0.76766595567255402</v>
+      </c>
+      <c r="I4" s="29">
+        <v>0.78015663317693795</v>
+      </c>
+      <c r="J4" s="30">
+        <v>0.772899779649726</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
+      <c r="C5" s="31">
+        <v>0.60593089556964796</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.539743373789491</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0.61141819401573405</v>
+      </c>
+      <c r="F5" s="31">
+        <v>0.75846315025511502</v>
+      </c>
+      <c r="G5" s="31">
+        <v>0.78472907446790996</v>
+      </c>
+      <c r="H5" s="31">
+        <v>0.75421215686387399</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0.60632914717966302</v>
+      </c>
+      <c r="J5" s="32">
+        <v>0.60526864013858905</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
+      <c r="C6" s="31">
+        <v>0.62174888042751197</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.76713222673674397</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0.76417245023257696</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.76967354833594204</v>
+      </c>
+      <c r="G6" s="31">
+        <v>0.78307854354320405</v>
+      </c>
+      <c r="H6" s="31">
+        <v>0.76945083229450295</v>
+      </c>
+      <c r="I6" s="31">
+        <v>0.76266274009255397</v>
+      </c>
+      <c r="J6" s="32">
+        <v>0.65283217859920495</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -2437,57 +3404,105 @@
       <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
+      <c r="C7" s="31">
+        <v>0.619863623631696</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.76063086606805896</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.76301854227561094</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.77477806775574298</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.74882092124532296</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0.78730747151664404</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0.77311089997151905</v>
+      </c>
+      <c r="J7" s="32">
+        <v>0.76437299232675704</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="31">
+        <v>0.61728538524973897</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.61042471849954405</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0.61124443238812398</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0.75325503154455298</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.61379009126050699</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0.60180026270551301</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0.71028586246543701</v>
+      </c>
+      <c r="J8" s="32">
+        <v>0.61783454315483799</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="C9" s="33">
+        <v>0.60062878804722397</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.75321658362702404</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0.76846313558534196</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0.75539295687233599</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.771269192420037</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0.75770038564748599</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0.75649659613539699</v>
+      </c>
+      <c r="J9" s="34">
+        <v>0.76677162348467798</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -2528,42 +3543,90 @@
       <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="C13" s="29">
+        <v>0.72039622404238901</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.77945979850376701</v>
+      </c>
+      <c r="E13" s="29">
+        <v>0.78328461938654403</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0.77107403843088496</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0.78070145093117904</v>
+      </c>
+      <c r="H13" s="29">
+        <v>0.78143686689847203</v>
+      </c>
+      <c r="I13" s="29">
+        <v>0.77711911586105398</v>
+      </c>
+      <c r="J13" s="30">
+        <v>0.78069480772639499</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="C14" s="31">
+        <v>0.59798872917264301</v>
+      </c>
+      <c r="D14" s="31">
+        <v>0.78606731867824498</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.611736789270656</v>
+      </c>
+      <c r="F14" s="31">
+        <v>0.74496955183081803</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.75422936311298705</v>
+      </c>
+      <c r="H14" s="31">
+        <v>0.77039714090852096</v>
+      </c>
+      <c r="I14" s="31">
+        <v>0.61137995514800803</v>
+      </c>
+      <c r="J14" s="32">
+        <v>0.60944182571554595</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="C15" s="31">
+        <v>0.61754564299216297</v>
+      </c>
+      <c r="D15" s="31">
+        <v>0.64133264599404505</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.77313107009787196</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.76070041431226498</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.65550679550550095</v>
+      </c>
+      <c r="H15" s="31">
+        <v>0.78348240136780201</v>
+      </c>
+      <c r="I15" s="31">
+        <v>0.64267477229109804</v>
+      </c>
+      <c r="J15" s="32">
+        <v>0.80836342396848204</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
@@ -2572,42 +3635,90 @@
       <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
+      <c r="C16" s="31">
+        <v>0.70720322855220297</v>
+      </c>
+      <c r="D16" s="31">
+        <v>0.71783530829589204</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.74913657748302698</v>
+      </c>
+      <c r="F16" s="31">
+        <v>0.63460752601241199</v>
+      </c>
+      <c r="G16" s="31">
+        <v>0.74499783482306603</v>
+      </c>
+      <c r="H16" s="31">
+        <v>0.69455673641559801</v>
+      </c>
+      <c r="I16" s="31">
+        <v>0.71555053053632001</v>
+      </c>
+      <c r="J16" s="32">
+        <v>0.64126099848797502</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="C17" s="31">
+        <v>0.61314872136518395</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.61146545774876804</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0.60224976089358395</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.59619186370807997</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.60821083079189298</v>
+      </c>
+      <c r="H17" s="31">
+        <v>0.60070195234958002</v>
+      </c>
+      <c r="I17" s="31">
+        <v>0.61522451073358697</v>
+      </c>
+      <c r="J17" s="32">
+        <v>0.62916997976008004</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
+      <c r="C18" s="33">
+        <v>0.62326313868963601</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0.62100689088692396</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0.61859082818961797</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0.71677274165608396</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0.61352000849389698</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0.62428389599225598</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0.62544528860359805</v>
+      </c>
+      <c r="J18" s="34">
+        <v>0.74171085257513003</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2622,9 +3733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B47BB03-5D51-4927-8C90-D8C37E699AAE}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:J18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2634,18 +3743,18 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -2686,42 +3795,90 @@
       <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25"/>
+      <c r="C4" s="29">
+        <v>0.48580999890915899</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.68500200100675102</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.69230187092655004</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0.67301455209619399</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0.68834750372521702</v>
+      </c>
+      <c r="H4" s="29">
+        <v>0.68418168671860602</v>
+      </c>
+      <c r="I4" s="29">
+        <v>0.70778451075415505</v>
+      </c>
+      <c r="J4" s="30">
+        <v>0.70775403149117599</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
+      <c r="C5" s="31">
+        <v>0.48479263013877699</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.51919973072791503</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0.48122643422517603</v>
+      </c>
+      <c r="F5" s="31">
+        <v>0.67041110475305299</v>
+      </c>
+      <c r="G5" s="31">
+        <v>0.72956080513936705</v>
+      </c>
+      <c r="H5" s="31">
+        <v>0.69647899731268004</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0.47975460890099197</v>
+      </c>
+      <c r="J5" s="32">
+        <v>0.48834435737343901</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
+      <c r="C6" s="31">
+        <v>0.59065411871507101</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.69778377207819298</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0.68900548681965201</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.68601717688018504</v>
+      </c>
+      <c r="G6" s="31">
+        <v>0.71725586335157598</v>
+      </c>
+      <c r="H6" s="31">
+        <v>0.71292995212451304</v>
+      </c>
+      <c r="I6" s="31">
+        <v>0.69056466545844597</v>
+      </c>
+      <c r="J6" s="32">
+        <v>0.72745735435564096</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -2730,57 +3887,105 @@
       <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
+      <c r="C7" s="31">
+        <v>0.50124484528207003</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.69189791717859594</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.68247669093874697</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.68883082028420795</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.656087924944323</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0.70938399137240205</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0.69423012215336599</v>
+      </c>
+      <c r="J7" s="32">
+        <v>0.68855070198414003</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="31">
+        <v>0.57470532171149802</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.483094263955964</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0.48586027877848498</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0.67163930388955995</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.480498200613517</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0.46741460663216799</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0.60938883221676898</v>
+      </c>
+      <c r="J8" s="32">
+        <v>0.49720869947588098</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="C9" s="33">
+        <v>0.571435611618485</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.69559103837853398</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0.70259114591268002</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0.67435462464852003</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.69585210187350299</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0.66983343065960899</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0.67872187292478903</v>
+      </c>
+      <c r="J9" s="34">
+        <v>0.68261786230088795</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -2821,42 +4026,90 @@
       <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="C13" s="29">
+        <v>0.63854095207524697</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.70010164499657501</v>
+      </c>
+      <c r="E13" s="29">
+        <v>0.71456381973252803</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0.69781972581515195</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0.70574414708656696</v>
+      </c>
+      <c r="H13" s="29">
+        <v>0.71095714072967897</v>
+      </c>
+      <c r="I13" s="29">
+        <v>0.70002815735457702</v>
+      </c>
+      <c r="J13" s="30">
+        <v>0.71957827950853503</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="C14" s="31">
+        <v>0.56566804686085004</v>
+      </c>
+      <c r="D14" s="31">
+        <v>0.72555707363910205</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.48438960861402602</v>
+      </c>
+      <c r="F14" s="31">
+        <v>0.66063116276377798</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.68456432089355801</v>
+      </c>
+      <c r="H14" s="31">
+        <v>0.70329187314470398</v>
+      </c>
+      <c r="I14" s="31">
+        <v>0.48631300669919802</v>
+      </c>
+      <c r="J14" s="32">
+        <v>0.61560850257572497</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="C15" s="31">
+        <v>0.60574045008789001</v>
+      </c>
+      <c r="D15" s="31">
+        <v>0.70484902162723095</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.70904910980150404</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.68147035891282104</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.70026989662205297</v>
+      </c>
+      <c r="H15" s="31">
+        <v>0.71552493584032695</v>
+      </c>
+      <c r="I15" s="31">
+        <v>0.69603850098367803</v>
+      </c>
+      <c r="J15" s="32">
+        <v>0.73834863580003196</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
@@ -2865,42 +4118,90 @@
       <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
+      <c r="C16" s="31">
+        <v>0.60761806839973398</v>
+      </c>
+      <c r="D16" s="31">
+        <v>0.62113700155858798</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.65130895497890795</v>
+      </c>
+      <c r="F16" s="31">
+        <v>0.51642277473200804</v>
+      </c>
+      <c r="G16" s="31">
+        <v>0.65370460754764603</v>
+      </c>
+      <c r="H16" s="31">
+        <v>0.60657816222457595</v>
+      </c>
+      <c r="I16" s="31">
+        <v>0.62091075481490698</v>
+      </c>
+      <c r="J16" s="32">
+        <v>0.51937597439937599</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="C17" s="31">
+        <v>0.60094977607002698</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.59730325098800596</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0.57929869963114999</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.56973421652396905</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.60245442540891203</v>
+      </c>
+      <c r="H17" s="31">
+        <v>0.58702988430775405</v>
+      </c>
+      <c r="I17" s="31">
+        <v>0.59288707254563899</v>
+      </c>
+      <c r="J17" s="32">
+        <v>0.61492514221426897</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
+      <c r="C18" s="33">
+        <v>0.62466946231800502</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0.59729188519642396</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0.59751516098500301</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0.62187803489251103</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0.60211121507797805</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0.63523903969254403</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0.59325812352371998</v>
+      </c>
+      <c r="J18" s="34">
+        <v>0.64018629477590006</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
adjusted xls of motor faiulre files
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_wallFollow_01_hold_02.xlsx
+++ b/results_analysis/ksom_wallFollow_01_hold_02.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C2ADC-DF28-4E39-A66A-C13EF03722A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECF86C6-47F8-4D8B-A737-73F72EF66FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView minimized="1" xWindow="20175" yWindow="1560" windowWidth="11520" windowHeight="7875" activeTab="1" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="hp_best" sheetId="7" r:id="rId1"/>
-    <sheet name="acc_max" sheetId="1" r:id="rId2"/>
+    <sheet name="acc_best" sheetId="1" r:id="rId2"/>
     <sheet name="acc_mean" sheetId="2" r:id="rId3"/>
     <sheet name="acc_median" sheetId="5" r:id="rId4"/>
     <sheet name="acc_std" sheetId="6" r:id="rId5"/>
@@ -935,18 +935,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -977,7 +977,7 @@
       </c>
       <c r="O2" s="47"/>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -1161,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -1253,7 +1253,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -1313,20 +1313,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A889A0D-6079-4851-A2AA-AD4BB1CBB64D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
@@ -1340,7 +1340,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>0.808810572687225</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -1434,7 +1434,7 @@
         <v>0.61167400881057299</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -1464,7 +1464,7 @@
         <v>0.82863436123348</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>0.798017621145374</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -1526,7 +1526,7 @@
         <v>0.61740088105726898</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -1556,8 +1556,8 @@
         <v>0.79295154185021999</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="I11" s="46"/>
       <c r="J11" s="47"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>0.81497797356828205</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -1665,7 +1665,7 @@
         <v>0.76453744493392095</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -1695,7 +1695,7 @@
         <v>0.83237885462555095</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>0.63480176211453698</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -1757,7 +1757,7 @@
         <v>0.764096916299559</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -1802,15 +1802,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
@@ -1824,7 +1824,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>0.73321585903083697</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="42"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -1918,7 +1918,7 @@
         <v>0.475594713656388</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -1948,7 +1948,7 @@
         <v>0.74870044052863405</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>2</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>0.74707048458149805</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -2010,7 +2010,7 @@
         <v>0.44079295154185</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="43"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -2040,8 +2040,8 @@
         <v>0.75229074889867797</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
@@ -2055,7 +2055,7 @@
       <c r="I11" s="46"/>
       <c r="J11" s="47"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>0.77146916299559498</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -2149,7 +2149,7 @@
         <v>0.50853964757709302</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -2179,7 +2179,7 @@
         <v>0.603665198237885</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0.60542731277533102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -2241,7 +2241,7 @@
         <v>0.50255286343612304</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -2286,14 +2286,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
@@ -2307,7 +2307,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>0.75308370044052897</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -2401,7 +2401,7 @@
         <v>0.55517621145374396</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -2431,7 +2431,7 @@
         <v>0.77444933920704795</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>0.77709251101321597</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -2493,7 +2493,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -2523,8 +2523,8 @@
         <v>0.75892070484581498</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
@@ -2538,7 +2538,7 @@
       <c r="I11" s="46"/>
       <c r="J11" s="47"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>0.78116740088105696</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -2632,7 +2632,7 @@
         <v>0.54063876651982401</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -2662,7 +2662,7 @@
         <v>0.60704845814978003</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>0.61057268722466995</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -2724,7 +2724,7 @@
         <v>0.45638766519823798</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -2769,14 +2769,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
@@ -2790,7 +2790,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>6.43209353935211E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -2884,7 +2884,7 @@
         <v>0.173934251701958</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -2914,7 +2914,7 @@
         <v>8.7806973294354995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>7.9679958379958601E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -2976,7 +2976,7 @@
         <v>0.148471831245376</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -3006,8 +3006,8 @@
         <v>3.3138569484302702E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="I11" s="46"/>
       <c r="J11" s="47"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>4.06699040450198E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -3115,7 +3115,7 @@
         <v>0.149088005815424</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -3145,7 +3145,7 @@
         <v>0.119481264849919</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>2.1485105342414001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -3207,7 +3207,7 @@
         <v>0.129166579408311</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -3252,14 +3252,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>0.772899779649726</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -3367,7 +3367,7 @@
         <v>0.60526864013858905</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -3397,7 +3397,7 @@
         <v>0.65283217859920495</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>0.76437299232675704</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -3459,7 +3459,7 @@
         <v>0.61783454315483799</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -3489,8 +3489,8 @@
         <v>0.76677162348467798</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="I11" s="46"/>
       <c r="J11" s="47"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>0.78069480772639499</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -3598,7 +3598,7 @@
         <v>0.60944182571554595</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -3628,7 +3628,7 @@
         <v>0.80836342396848204</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>0.64126099848797502</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -3690,7 +3690,7 @@
         <v>0.62916997976008004</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -3733,16 +3733,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B47BB03-5D51-4927-8C90-D8C37E699AAE}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
@@ -3756,7 +3758,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3788,7 +3790,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -3820,7 +3822,7 @@
         <v>0.70775403149117599</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -3850,7 +3852,7 @@
         <v>0.48834435737343901</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -3880,7 +3882,7 @@
         <v>0.72745735435564096</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3912,7 +3914,7 @@
         <v>0.68855070198414003</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -3942,7 +3944,7 @@
         <v>0.49720869947588098</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -3972,8 +3974,8 @@
         <v>0.68261786230088795</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>20</v>
       </c>
@@ -3987,7 +3989,7 @@
       <c r="I11" s="46"/>
       <c r="J11" s="47"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -4019,7 +4021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -4051,7 +4053,7 @@
         <v>0.71957827950853503</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -4081,7 +4083,7 @@
         <v>0.61560850257572497</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -4111,7 +4113,7 @@
         <v>0.73834863580003196</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -4143,7 +4145,7 @@
         <v>0.51937597439937599</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -4173,7 +4175,7 @@
         <v>0.61492514221426897</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>

</xml_diff>